<commit_message>
Şampiyon yazısı ve animasyonu eklendi
</commit_message>
<xml_diff>
--- a/data/playoff-sonuclari.xlsx
+++ b/data/playoff-sonuclari.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F220C0D1-F1B7-48F3-BF18-8AEE0B53165B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FF84E4-6DFF-4F67-9BAA-0EACB200FDE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5700" yWindow="2205" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Playoff" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
   <si>
     <t>Maç Türü</t>
   </si>
@@ -476,7 +476,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -693,9 +693,6 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
       <c r="F15" s="1">
         <v>45852</v>
       </c>
@@ -793,7 +790,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:G2 A4:C5 C3 A7:C8 C6 A10:C11 C9 A13:C14 C12 A16:A17 C15 A19:A20 C18 A22:A23 C21 C24 C16:C17 C19:C20 C22:C23" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G2 A4:C5 C3 A7:C8 C6 A10:C11 C9 A13:C14 C12 A16:A17 A19:A20 C18 A22:A23 C21 C24 C16:C17 C19:C20 C22:C23" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
07.07.2025 - maç sonuçları eklendi
</commit_message>
<xml_diff>
--- a/data/playoff-sonuclari.xlsx
+++ b/data/playoff-sonuclari.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FF84E4-6DFF-4F67-9BAA-0EACB200FDE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C3ECAF-39CC-4A66-9756-E7C59C1AD2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="2205" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Playoff" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="25">
   <si>
     <t>Maç Türü</t>
   </si>
@@ -476,7 +476,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -544,6 +544,12 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
       <c r="F3" s="1">
         <v>45845</v>
       </c>
@@ -583,6 +589,12 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
       <c r="F6" s="1">
         <v>45845</v>
       </c>
@@ -693,6 +705,12 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
       <c r="F15" s="1">
         <v>45852</v>
       </c>

</xml_diff>

<commit_message>
Araklı 1961 Spor vs Çirihtalar - Maç Sonucu eklendi
</commit_message>
<xml_diff>
--- a/data/playoff-sonuclari.xlsx
+++ b/data/playoff-sonuclari.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C3ECAF-39CC-4A66-9756-E7C59C1AD2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB46B45E-D307-4DAB-89ED-A154662BB61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Playoff" sheetId="1" r:id="rId1"/>
@@ -476,7 +476,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -634,6 +634,12 @@
       <c r="C9" t="s">
         <v>8</v>
       </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
       <c r="F9" s="1">
         <v>45847</v>
       </c>

</xml_diff>

<commit_message>
09.07.2027 - Maç Kayıtları eklendi
</commit_message>
<xml_diff>
--- a/data/playoff-sonuclari.xlsx
+++ b/data/playoff-sonuclari.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1DA7F7-4F93-4DE9-8765-80CD0AFC7B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC450CC-F974-4800-82CB-5B7DF57185F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2955" yWindow="1890" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Playoff" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="31">
   <si>
     <t>Maç Türü</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>https://youtu.be/pssuvQr70gs</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Zc2rrwS6Ccw</t>
+  </si>
+  <si>
+    <t>https://youtu.be/7p5q1Q6-Q6w</t>
   </si>
 </sst>
 </file>
@@ -488,7 +494,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -671,6 +677,9 @@
       <c r="G9" s="2">
         <v>0.875</v>
       </c>
+      <c r="K9" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -721,6 +730,9 @@
       </c>
       <c r="J12">
         <v>2</v>
+      </c>
+      <c r="K12" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
prod - sosyal medya hesapları eklendi
</commit_message>
<xml_diff>
--- a/data/playoff-sonuclari.xlsx
+++ b/data/playoff-sonuclari.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A1D743-30B5-42AB-8D47-ED77F5AF8DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A4DE14-65E2-4470-9978-BC05FFCF08FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -494,7 +494,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
14.07.2025 maçlarının saatleri güncellendi. Sosyal medya iconlarının yönü değişti
</commit_message>
<xml_diff>
--- a/data/playoff-sonuclari.xlsx
+++ b/data/playoff-sonuclari.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A4DE14-65E2-4470-9978-BC05FFCF08FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F67E4F9-D57E-4702-A216-EBF68764FB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Playoff" sheetId="1" r:id="rId1"/>
@@ -494,7 +494,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -770,7 +770,7 @@
         <v>45852</v>
       </c>
       <c r="G15" s="2">
-        <v>0.875</v>
+        <v>0.91666666666666663</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -805,7 +805,7 @@
         <v>45852</v>
       </c>
       <c r="G18" s="2">
-        <v>0.91666666666666663</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
15.07.2025 - maç sonuçları eklendi
</commit_message>
<xml_diff>
--- a/data/playoff-sonuclari.xlsx
+++ b/data/playoff-sonuclari.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F67E4F9-D57E-4702-A216-EBF68764FB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AAB4EA-B147-4B23-AB7A-3DAD69802207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="31">
   <si>
     <t>Maç Türü</t>
   </si>
@@ -494,7 +494,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -766,12 +766,24 @@
       <c r="B15" t="s">
         <v>18</v>
       </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
       <c r="F15" s="1">
         <v>45852</v>
       </c>
       <c r="G15" s="2">
         <v>0.91666666666666663</v>
       </c>
+      <c r="I15">
+        <v>11</v>
+      </c>
+      <c r="J15">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -782,7 +794,7 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -791,7 +803,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -801,14 +813,26 @@
       <c r="C18" t="s">
         <v>8</v>
       </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
       <c r="F18" s="1">
         <v>45852</v>
       </c>
       <c r="G18" s="2">
         <v>0.875</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>12</v>
+      </c>
+      <c r="J18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -817,7 +841,7 @@
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -826,7 +850,13 @@
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
       <c r="C21" t="s">
         <v>8</v>
       </c>
@@ -837,7 +867,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -846,7 +876,7 @@
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -855,7 +885,13 @@
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
       <c r="C24" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
yari final mac goruntuleri eklendi
</commit_message>
<xml_diff>
--- a/data/playoff-sonuclari.xlsx
+++ b/data/playoff-sonuclari.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AAB4EA-B147-4B23-AB7A-3DAD69802207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E39FC1-1F3D-4D5C-B0ED-DA85D1D805BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="33">
   <si>
     <t>Maç Türü</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>https://youtu.be/7p5q1Q6-Q6w</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Yp_pg2vCASI</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Dtif43f-0tQ</t>
   </si>
 </sst>
 </file>
@@ -494,7 +500,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -784,6 +790,9 @@
       <c r="J15">
         <v>10</v>
       </c>
+      <c r="K15" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -794,7 +803,7 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -803,7 +812,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -831,8 +840,11 @@
       <c r="J18">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -841,7 +853,7 @@
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -850,7 +862,7 @@
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -867,7 +879,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -876,7 +888,7 @@
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -885,7 +897,7 @@
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
final ve 3.lük maç sonuçları eklendi
</commit_message>
<xml_diff>
--- a/data/playoff-sonuclari.xlsx
+++ b/data/playoff-sonuclari.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E39FC1-1F3D-4D5C-B0ED-DA85D1D805BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC0985E-FDE8-4D71-A873-4F757D697968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Playoff" sheetId="1" r:id="rId1"/>
@@ -500,7 +500,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -872,6 +872,12 @@
       <c r="C21" t="s">
         <v>8</v>
       </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
       <c r="F21" s="1">
         <v>45857</v>
       </c>
@@ -906,6 +912,12 @@
       </c>
       <c r="C24" t="s">
         <v>8</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
       </c>
       <c r="F24" s="1">
         <v>45857</v>

</xml_diff>

<commit_message>
final ve üçüncülük maçı görüntüleri eklendi, 3.lük maçı skoru düzeltildi
</commit_message>
<xml_diff>
--- a/data/playoff-sonuclari.xlsx
+++ b/data/playoff-sonuclari.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC0985E-FDE8-4D71-A873-4F757D697968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C199D683-B70B-4936-A376-BA514FB16E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="35">
   <si>
     <t>Maç Türü</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>https://youtu.be/Dtif43f-0tQ</t>
+  </si>
+  <si>
+    <t>https://youtu.be/UwPkIRGWSeA</t>
+  </si>
+  <si>
+    <t>https://youtu.be/v4QNOTOEC-E</t>
   </si>
 </sst>
 </file>
@@ -500,7 +506,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -884,6 +890,9 @@
       <c r="G21" s="2">
         <v>0.91666666666666663</v>
       </c>
+      <c r="K21" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -914,7 +923,7 @@
         <v>8</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E24">
         <v>2</v>
@@ -924,6 +933,9 @@
       </c>
       <c r="G24" s="2">
         <v>0.875</v>
+      </c>
+      <c r="K24" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3.lük maçı skoru ve linki güncellendi
</commit_message>
<xml_diff>
--- a/data/playoff-sonuclari.xlsx
+++ b/data/playoff-sonuclari.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yakay\OneDrive\Masaüstü\d-8-ligi\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C199D683-B70B-4936-A376-BA514FB16E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862887E7-E143-4438-922E-62CDA443FB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Playoff" sheetId="1" r:id="rId1"/>
@@ -124,7 +124,7 @@
     <t>https://youtu.be/UwPkIRGWSeA</t>
   </si>
   <si>
-    <t>https://youtu.be/v4QNOTOEC-E</t>
+    <t>https://youtu.be/Y2WH_2cX65g</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -923,7 +923,7 @@
         <v>8</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E24">
         <v>2</v>

</xml_diff>